<commit_message>
Blog page crud opration fix
</commit_message>
<xml_diff>
--- a/Pending Task in AdminPanel (chintamani db).xlsx
+++ b/Pending Task in AdminPanel (chintamani db).xlsx
@@ -1,19 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\website-chintamani-latest\website-chintamani\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\website-chintamani\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10B7F365-FEDD-4112-B1F3-49BD7661FDF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C304AEB2-BC69-4478-92FE-5B742BFE9BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{13732B57-96E7-4933-9FF4-EDB4A3E44D40}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{13732B57-96E7-4933-9FF4-EDB4A3E44D40}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="tasks" sheetId="2" r:id="rId1"/>
+    <sheet name="Images" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
   <si>
     <t>Leasing Page</t>
   </si>
@@ -90,13 +92,115 @@
   </si>
   <si>
     <t xml:space="preserve"> Note :text area value not fetched needs to be fixed in admin panel</t>
+  </si>
+  <si>
+    <t>Task</t>
+  </si>
+  <si>
+    <t>Side</t>
+  </si>
+  <si>
+    <t>Page</t>
+  </si>
+  <si>
+    <t>Image upload error message display</t>
+  </si>
+  <si>
+    <t>Adminside</t>
+  </si>
+  <si>
+    <t>All pages</t>
+  </si>
+  <si>
+    <t>On click of delete button remove the image</t>
+  </si>
+  <si>
+    <t>AdminSide</t>
+  </si>
+  <si>
+    <t>add_Interior</t>
+  </si>
+  <si>
+    <t>Change title for SEO add</t>
+  </si>
+  <si>
+    <t>Alias check functionality</t>
+  </si>
+  <si>
+    <t>SEO details replace the field name</t>
+  </si>
+  <si>
+    <t>Image no</t>
+  </si>
+  <si>
+    <t>img1</t>
+  </si>
+  <si>
+    <t>Bredcrumb changes</t>
+  </si>
+  <si>
+    <t>edit_interior</t>
+  </si>
+  <si>
+    <t>Gallary image error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Required field </t>
+  </si>
+  <si>
+    <t>Pagination</t>
+  </si>
+  <si>
+    <t>interiors</t>
+  </si>
+  <si>
+    <t>Blogs</t>
+  </si>
+  <si>
+    <t>Column change</t>
+  </si>
+  <si>
+    <t>img2</t>
+  </si>
+  <si>
+    <t>Add blog</t>
+  </si>
+  <si>
+    <t>image3</t>
+  </si>
+  <si>
+    <t>Edit Blog</t>
+  </si>
+  <si>
+    <t>imageupdate in blog edit is not working</t>
+  </si>
+  <si>
+    <t>Bredcrum captilization</t>
+  </si>
+  <si>
+    <t>Aminiies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delete aminities </t>
+  </si>
+  <si>
+    <t>Session management</t>
+  </si>
+  <si>
+    <t>Sidebar is not sticking all time</t>
+  </si>
+  <si>
+    <t>Sidebar</t>
+  </si>
+  <si>
+    <t>Add required field maek</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +218,22 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -136,24 +256,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -167,6 +288,143 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>484495</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>66333</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{458675F3-1F3A-8544-62AC-A1A0B6164432}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="10238095" cy="2733333"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>227276</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>113643</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{9DA27BA5-179F-B2AB-5C1F-0F61575706B9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="3048000"/>
+          <a:ext cx="10590476" cy="5257143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>599314</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>190262</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="5" name="Picture 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5402F792-E2A4-85C9-2F1B-108C13C1141C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="8763000"/>
+          <a:ext cx="6085714" cy="1904762"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -465,39 +723,351 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{298D0B0F-40BB-45D0-9131-D61CC7406483}">
+  <dimension ref="A1:D23"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="36.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" t="s">
+        <v>26</v>
+      </c>
+      <c r="C8" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" t="s">
+        <v>26</v>
+      </c>
+      <c r="C11" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>36</v>
+      </c>
+      <c r="B12" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>37</v>
+      </c>
+      <c r="B13" t="s">
+        <v>26</v>
+      </c>
+      <c r="C13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" t="s">
+        <v>26</v>
+      </c>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>40</v>
+      </c>
+      <c r="B15" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" t="s">
+        <v>39</v>
+      </c>
+      <c r="D15" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" t="s">
+        <v>42</v>
+      </c>
+      <c r="D16" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>46</v>
+      </c>
+      <c r="B18" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>48</v>
+      </c>
+      <c r="B19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>37</v>
+      </c>
+      <c r="B20" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>49</v>
+      </c>
+      <c r="B21" t="s">
+        <v>26</v>
+      </c>
+      <c r="C21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B22" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>52</v>
+      </c>
+      <c r="B23" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" t="s">
+        <v>24</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A4" location="Sheet3!A1" display="Change title for SEO add" xr:uid="{D60951E9-9E15-4ACF-98F1-D8D4AD9FB3D7}"/>
+    <hyperlink ref="A9" location="Sheet3!A1" display="Change title for SEO add" xr:uid="{478E3ABA-ED38-4223-B9D3-D42A6ABBD772}"/>
+    <hyperlink ref="A16" location="Sheet3!A1" display="Change title for SEO add" xr:uid="{1B77D8A5-F6C7-497E-A691-6C88B445AE26}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8774A6B8-252A-48D9-91C6-63EFAB2C2B50}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8205788-B303-4176-92CC-83B5DE68E184}">
   <dimension ref="A1:L13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.5546875" customWidth="1"/>
-    <col min="4" max="4" width="33.77734375" customWidth="1"/>
-    <col min="6" max="6" width="39.33203125" customWidth="1"/>
-    <col min="8" max="8" width="35.21875" customWidth="1"/>
-    <col min="10" max="10" width="11.77734375" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="4" max="4" width="33.7109375" customWidth="1"/>
+    <col min="6" max="6" width="39.28515625" customWidth="1"/>
+    <col min="8" max="8" width="35.28515625" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
-      <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
-      <c r="J1" s="3"/>
-      <c r="K1" s="3"/>
-      <c r="L1" s="3"/>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -517,81 +1087,81 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="C3" s="5" t="s">
+      <c r="B3" s="5"/>
+      <c r="C3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5" t="s">
+      <c r="D3" s="6"/>
+      <c r="E3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5" t="s">
+      <c r="F3" s="6"/>
+      <c r="G3" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5" t="s">
+      <c r="H3" s="6"/>
+      <c r="I3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="J3" s="5"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="J3" s="6"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="C4" s="5" t="s">
+      <c r="B4" s="5"/>
+      <c r="C4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5" t="s">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5" t="s">
+      <c r="F4" s="6"/>
+      <c r="G4" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="H4" s="5"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
+      <c r="H4" s="6"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="3"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
+      <c r="B5" s="5"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="3"/>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="B6" s="5"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B7" s="4"/>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
+      <c r="B7" s="5"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="B8" s="5"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
pending task sheet updated
</commit_message>
<xml_diff>
--- a/Pending Task in AdminPanel (chintamani db).xlsx
+++ b/Pending Task in AdminPanel (chintamani db).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\website-chintamani\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\website-chintamani-latest\website-chintamani\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C304AEB2-BC69-4478-92FE-5B742BFE9BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FC83EA-37C5-4714-B51B-8E6E16F6072E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{13732B57-96E7-4933-9FF4-EDB4A3E44D40}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{13732B57-96E7-4933-9FF4-EDB4A3E44D40}"/>
   </bookViews>
   <sheets>
     <sheet name="tasks" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
   <si>
     <t>Leasing Page</t>
   </si>
@@ -194,6 +194,21 @@
   </si>
   <si>
     <t>Add required field maek</t>
+  </si>
+  <si>
+    <t>addblog not working</t>
+  </si>
+  <si>
+    <t>edit blog not working</t>
+  </si>
+  <si>
+    <t xml:space="preserve">amenities add </t>
+  </si>
+  <si>
+    <t>add_interior page not found need to be fixed</t>
+  </si>
+  <si>
+    <t>edit_interior functionality not working</t>
   </si>
 </sst>
 </file>
@@ -724,20 +739,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{298D0B0F-40BB-45D0-9131-D61CC7406483}">
-  <dimension ref="A1:D23"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.5703125" customWidth="1"/>
-    <col min="2" max="2" width="20.140625" customWidth="1"/>
-    <col min="3" max="3" width="33.28515625" customWidth="1"/>
+    <col min="1" max="1" width="36.5546875" customWidth="1"/>
+    <col min="2" max="2" width="20.109375" customWidth="1"/>
+    <col min="3" max="3" width="33.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -751,7 +766,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -762,7 +777,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -773,7 +788,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -787,7 +802,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -798,7 +813,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -812,7 +827,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -823,7 +838,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -834,7 +849,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
@@ -845,7 +860,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -856,7 +871,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -867,7 +882,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -878,7 +893,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -889,7 +904,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -903,7 +918,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -917,7 +932,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
         <v>28</v>
       </c>
@@ -931,7 +946,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -942,7 +957,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -953,7 +968,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -964,7 +979,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -975,7 +990,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -986,7 +1001,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -997,7 +1012,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -1006,6 +1021,31 @@
       </c>
       <c r="C23" t="s">
         <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1027,7 +1067,7 @@
       <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1042,16 +1082,16 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.5703125" customWidth="1"/>
-    <col min="4" max="4" width="33.7109375" customWidth="1"/>
-    <col min="6" max="6" width="39.28515625" customWidth="1"/>
-    <col min="8" max="8" width="35.28515625" customWidth="1"/>
-    <col min="10" max="10" width="11.7109375" customWidth="1"/>
+    <col min="2" max="2" width="23.5546875" customWidth="1"/>
+    <col min="4" max="4" width="33.6640625" customWidth="1"/>
+    <col min="6" max="6" width="39.33203125" customWidth="1"/>
+    <col min="8" max="8" width="35.33203125" customWidth="1"/>
+    <col min="10" max="10" width="11.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -1067,7 +1107,7 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1087,7 +1127,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -1109,7 +1149,7 @@
       </c>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -1127,41 +1167,41 @@
       </c>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="5"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="5"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B12" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
complete website and admin panel
</commit_message>
<xml_diff>
--- a/Pending Task in AdminPanel (chintamani db).xlsx
+++ b/Pending Task in AdminPanel (chintamani db).xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\website-chintamani-latest\website-chintamani\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\website-chintamani\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23FC83EA-37C5-4714-B51B-8E6E16F6072E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C304AEB2-BC69-4478-92FE-5B742BFE9BBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{13732B57-96E7-4933-9FF4-EDB4A3E44D40}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{13732B57-96E7-4933-9FF4-EDB4A3E44D40}"/>
   </bookViews>
   <sheets>
     <sheet name="tasks" sheetId="2" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="53">
   <si>
     <t>Leasing Page</t>
   </si>
@@ -194,21 +194,6 @@
   </si>
   <si>
     <t>Add required field maek</t>
-  </si>
-  <si>
-    <t>addblog not working</t>
-  </si>
-  <si>
-    <t>edit blog not working</t>
-  </si>
-  <si>
-    <t xml:space="preserve">amenities add </t>
-  </si>
-  <si>
-    <t>add_interior page not found need to be fixed</t>
-  </si>
-  <si>
-    <t>edit_interior functionality not working</t>
   </si>
 </sst>
 </file>
@@ -739,20 +724,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{298D0B0F-40BB-45D0-9131-D61CC7406483}">
-  <dimension ref="A1:D30"/>
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.5546875" customWidth="1"/>
-    <col min="2" max="2" width="20.109375" customWidth="1"/>
-    <col min="3" max="3" width="33.33203125" customWidth="1"/>
+    <col min="1" max="1" width="36.5703125" customWidth="1"/>
+    <col min="2" max="2" width="20.140625" customWidth="1"/>
+    <col min="3" max="3" width="33.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>19</v>
       </c>
@@ -766,7 +751,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -777,7 +762,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>25</v>
       </c>
@@ -788,7 +773,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>28</v>
       </c>
@@ -802,7 +787,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -813,7 +798,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -827,7 +812,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>33</v>
       </c>
@@ -838,7 +823,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>30</v>
       </c>
@@ -849,7 +834,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>28</v>
       </c>
@@ -860,7 +845,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>35</v>
       </c>
@@ -871,7 +856,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>36</v>
       </c>
@@ -882,7 +867,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>36</v>
       </c>
@@ -893,7 +878,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -904,7 +889,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>37</v>
       </c>
@@ -918,7 +903,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>40</v>
       </c>
@@ -932,7 +917,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>28</v>
       </c>
@@ -946,7 +931,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>45</v>
       </c>
@@ -957,7 +942,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>46</v>
       </c>
@@ -968,7 +953,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>48</v>
       </c>
@@ -979,7 +964,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>37</v>
       </c>
@@ -990,7 +975,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>49</v>
       </c>
@@ -1001,7 +986,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>50</v>
       </c>
@@ -1012,7 +997,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>52</v>
       </c>
@@ -1021,31 +1006,6 @@
       </c>
       <c r="C23" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1067,7 +1027,7 @@
       <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -1082,16 +1042,16 @@
       <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="23.5546875" customWidth="1"/>
-    <col min="4" max="4" width="33.6640625" customWidth="1"/>
-    <col min="6" max="6" width="39.33203125" customWidth="1"/>
-    <col min="8" max="8" width="35.33203125" customWidth="1"/>
-    <col min="10" max="10" width="11.6640625" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" customWidth="1"/>
+    <col min="4" max="4" width="33.7109375" customWidth="1"/>
+    <col min="6" max="6" width="39.28515625" customWidth="1"/>
+    <col min="8" max="8" width="35.28515625" customWidth="1"/>
+    <col min="10" max="10" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>6</v>
       </c>
@@ -1107,7 +1067,7 @@
       <c r="K1" s="5"/>
       <c r="L1" s="5"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1127,7 +1087,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>7</v>
       </c>
@@ -1149,7 +1109,7 @@
       </c>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
         <v>8</v>
       </c>
@@ -1167,41 +1127,41 @@
       </c>
       <c r="H4" s="6"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="5"/>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="5"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B7" s="5"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="5"/>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>18</v>
       </c>

</xml_diff>